<commit_message>
All recent models run and same basic polling error analysis done. Several tweaks to the model based on prelimary runs.
</commit_message>
<xml_diff>
--- a/python/Data/poll-data-sa.xlsx
+++ b/python/Data/poll-data-sa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\python\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D16B01-E61D-4CE4-B622-C712ADDB2E4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B47848-E912-47DB-A322-8E92B69C8209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7215" yWindow="3975" windowWidth="12465" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="2745" windowWidth="12570" windowHeight="16365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="17">
   <si>
     <t>MidDate</t>
   </si>
@@ -410,12 +410,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U149"/>
+  <dimension ref="A1:U148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A52"/>
+      <pane ySplit="600" topLeftCell="A58" activePane="bottomLeft"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="E62" sqref="E62"/>
+      <selection pane="bottomLeft" activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3152,25 +3152,25 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>43176</v>
+        <v>43540</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
       </c>
       <c r="C83">
-        <v>49.5</v>
+        <v>48</v>
       </c>
       <c r="D83">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E83" s="6">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F83" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G83" s="6">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H83" t="e">
         <v>#N/A</v>
@@ -3184,19 +3184,19 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>43540</v>
+        <v>43903</v>
       </c>
       <c r="B84" t="s">
         <v>8</v>
       </c>
       <c r="C84">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D84">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E84" s="6">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F84" s="6">
         <v>7</v>
@@ -3211,30 +3211,30 @@
         <v>#N/A</v>
       </c>
       <c r="J84" s="6">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>43903</v>
+        <v>44053</v>
       </c>
       <c r="B85" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C85">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D85">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E85" s="6">
-        <v>38</v>
-      </c>
-      <c r="F85" s="6">
-        <v>7</v>
-      </c>
-      <c r="G85" s="6">
-        <v>7</v>
+        <v>32</v>
+      </c>
+      <c r="F85" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G85" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H85" t="e">
         <v>#N/A</v>
@@ -3242,31 +3242,31 @@
       <c r="I85" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J85" s="6">
-        <v>5</v>
+      <c r="J85" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>44053</v>
+        <v>44092</v>
       </c>
       <c r="B86" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C86">
+        <v>47</v>
+      </c>
+      <c r="D86">
         <v>46</v>
       </c>
-      <c r="D86">
-        <v>44</v>
-      </c>
       <c r="E86" s="6">
-        <v>32</v>
-      </c>
-      <c r="F86" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G86" t="e">
-        <v>#N/A</v>
+        <v>35</v>
+      </c>
+      <c r="F86" s="6">
+        <v>10</v>
+      </c>
+      <c r="G86" s="6">
+        <v>5</v>
       </c>
       <c r="H86" t="e">
         <v>#N/A</v>
@@ -3274,47 +3274,15 @@
       <c r="I86" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J86" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
-        <v>44092</v>
-      </c>
-      <c r="B87" t="s">
-        <v>8</v>
-      </c>
-      <c r="C87">
-        <v>47</v>
-      </c>
-      <c r="D87">
-        <v>46</v>
-      </c>
-      <c r="E87" s="6">
-        <v>35</v>
-      </c>
-      <c r="F87" s="6">
-        <v>10</v>
-      </c>
-      <c r="G87" s="6">
-        <v>5</v>
-      </c>
-      <c r="H87" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I87" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J87" s="6">
+      <c r="J86" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I119" s="5"/>
-    </row>
-    <row r="149" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H149" s="4"/>
+    <row r="118" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I118" s="5"/>
+    </row>
+    <row r="148" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H148" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Projections more or less working now.
</commit_message>
<xml_diff>
--- a/python/Data/poll-data-sa.xlsx
+++ b/python/Data/poll-data-sa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\python\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B47848-E912-47DB-A322-8E92B69C8209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E97F79-F45F-4559-9F90-53BB75C740F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2745" windowWidth="12570" windowHeight="16365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="705" yWindow="7110" windowWidth="13200" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="17">
   <si>
     <t>MidDate</t>
   </si>
@@ -410,12 +410,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U148"/>
+  <dimension ref="A1:U147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A58" activePane="bottomLeft"/>
+      <pane ySplit="600" topLeftCell="A16" activePane="bottomLeft"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="B82" sqref="B82"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,22 +1936,22 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>41348</v>
+        <v>41590</v>
       </c>
       <c r="B45" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C45">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D45">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E45" s="6">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F45" s="6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G45" t="e">
         <v>#N/A</v>
@@ -1963,27 +1963,27 @@
         <v>#N/A</v>
       </c>
       <c r="J45">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>41590</v>
+        <v>41593</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C46">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D46">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E46" s="6">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F46" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G46" t="e">
         <v>#N/A</v>
@@ -1995,56 +1995,56 @@
         <v>#N/A</v>
       </c>
       <c r="J46">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>41593</v>
+        <v>41682</v>
       </c>
       <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>45</v>
+      </c>
+      <c r="D47">
+        <v>46</v>
+      </c>
+      <c r="E47" s="6">
+        <v>35</v>
+      </c>
+      <c r="F47" s="6">
+        <v>7</v>
+      </c>
+      <c r="G47" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H47" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I47" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J47">
         <v>12</v>
-      </c>
-      <c r="C47">
-        <v>47</v>
-      </c>
-      <c r="D47">
-        <v>40</v>
-      </c>
-      <c r="E47" s="6">
-        <v>33</v>
-      </c>
-      <c r="F47" s="6">
-        <v>10</v>
-      </c>
-      <c r="G47" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H47" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I47" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J47">
-        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>41682</v>
+        <v>41694</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C48">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D48">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E48" s="6">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F48" s="6">
         <v>7</v>
@@ -2059,27 +2059,27 @@
         <v>#N/A</v>
       </c>
       <c r="J48">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>41694</v>
+        <v>41710</v>
       </c>
       <c r="B49" t="s">
         <v>2</v>
       </c>
       <c r="C49">
-        <v>46</v>
+        <v>47.7</v>
       </c>
       <c r="D49">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E49" s="6">
         <v>34</v>
       </c>
       <c r="F49" s="6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G49" t="e">
         <v>#N/A</v>
@@ -2091,21 +2091,21 @@
         <v>#N/A</v>
       </c>
       <c r="J49">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>41710</v>
+        <v>41866</v>
       </c>
       <c r="B50" t="s">
         <v>2</v>
       </c>
       <c r="C50">
-        <v>47.7</v>
+        <v>51</v>
       </c>
       <c r="D50">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E50" s="6">
         <v>34</v>
@@ -2123,27 +2123,27 @@
         <v>#N/A</v>
       </c>
       <c r="J50">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>41866</v>
+        <v>41958</v>
       </c>
       <c r="B51" t="s">
         <v>2</v>
       </c>
       <c r="C51">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D51">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E51" s="6">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F51" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G51" t="e">
         <v>#N/A</v>
@@ -2155,24 +2155,24 @@
         <v>#N/A</v>
       </c>
       <c r="J51">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>41958</v>
+        <v>42050</v>
       </c>
       <c r="B52" t="s">
         <v>2</v>
       </c>
       <c r="C52">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D52">
         <v>33</v>
       </c>
       <c r="E52" s="6">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F52" s="6">
         <v>10</v>
@@ -2187,12 +2187,12 @@
         <v>#N/A</v>
       </c>
       <c r="J52">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>42050</v>
+        <v>42139</v>
       </c>
       <c r="B53" t="s">
         <v>2</v>
@@ -2224,22 +2224,22 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>42139</v>
+        <v>42221</v>
       </c>
       <c r="B54" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C54">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D54">
-        <v>33</v>
+        <v>39.5</v>
       </c>
       <c r="E54" s="6">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F54" s="6">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G54" t="e">
         <v>#N/A</v>
@@ -2251,24 +2251,24 @@
         <v>#N/A</v>
       </c>
       <c r="J54">
-        <v>21</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>42221</v>
+        <v>42246</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
       </c>
       <c r="C55">
-        <v>51</v>
+        <v>50.5</v>
       </c>
       <c r="D55">
         <v>39.5</v>
       </c>
       <c r="E55" s="6">
-        <v>34</v>
+        <v>33.5</v>
       </c>
       <c r="F55" s="6">
         <v>14</v>
@@ -2283,27 +2283,27 @@
         <v>#N/A</v>
       </c>
       <c r="J55">
-        <v>12.5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>42246</v>
+        <v>42288</v>
       </c>
       <c r="B56" t="s">
         <v>10</v>
       </c>
       <c r="C56">
-        <v>50.5</v>
+        <v>49</v>
       </c>
       <c r="D56">
-        <v>39.5</v>
+        <v>41.5</v>
       </c>
       <c r="E56" s="6">
         <v>33.5</v>
       </c>
       <c r="F56" s="6">
-        <v>14</v>
+        <v>12.5</v>
       </c>
       <c r="G56" t="e">
         <v>#N/A</v>
@@ -2311,31 +2311,31 @@
       <c r="H56" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I56" t="e">
-        <v>#N/A</v>
+      <c r="I56">
+        <v>5</v>
       </c>
       <c r="J56">
-        <v>13</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>42288</v>
+        <v>42323</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C57">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D57">
-        <v>41.5</v>
+        <v>32</v>
       </c>
       <c r="E57" s="6">
-        <v>33.5</v>
+        <v>39</v>
       </c>
       <c r="F57" s="6">
-        <v>12.5</v>
+        <v>10</v>
       </c>
       <c r="G57" t="e">
         <v>#N/A</v>
@@ -2343,66 +2343,66 @@
       <c r="H57" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I57">
-        <v>5</v>
+      <c r="I57" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J57">
-        <v>7.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>42323</v>
+        <v>42342</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C58">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D58">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E58" s="6">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F58" s="6">
         <v>10</v>
       </c>
-      <c r="G58" t="e">
-        <v>#N/A</v>
+      <c r="G58" s="6">
+        <v>18</v>
       </c>
       <c r="H58" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I58" t="e">
-        <v>#N/A</v>
+      <c r="I58">
+        <v>5.5</v>
       </c>
       <c r="J58">
-        <v>19</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>42342</v>
+        <v>42401</v>
       </c>
       <c r="B59" t="s">
         <v>10</v>
       </c>
       <c r="C59">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D59">
-        <v>37</v>
+        <v>35.5</v>
       </c>
       <c r="E59" s="6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F59" s="6">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="G59" s="6">
-        <v>18</v>
+        <v>20.5</v>
       </c>
       <c r="H59" t="e">
         <v>#N/A</v>
@@ -2411,62 +2411,62 @@
         <v>5.5</v>
       </c>
       <c r="J59">
-        <v>3.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>42401</v>
+        <v>42039</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C60">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D60">
-        <v>35.5</v>
+        <v>33</v>
       </c>
       <c r="E60" s="6">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F60" s="6">
-        <v>9.5</v>
+        <v>7</v>
       </c>
       <c r="G60" s="6">
-        <v>20.5</v>
+        <v>24</v>
       </c>
       <c r="H60" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I60">
-        <v>5.5</v>
+      <c r="I60" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J60">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>42039</v>
+        <v>42415</v>
       </c>
       <c r="B61" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C61">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D61">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E61" s="6">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F61" s="6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G61" s="6">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H61" t="e">
         <v>#N/A</v>
@@ -2475,7 +2475,7 @@
         <v>#N/A</v>
       </c>
       <c r="J61">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -2486,19 +2486,19 @@
         <v>4</v>
       </c>
       <c r="C62">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D62">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E62" s="6">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F62" s="6">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G62" s="6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H62" t="e">
         <v>#N/A</v>
@@ -2507,254 +2507,254 @@
         <v>#N/A</v>
       </c>
       <c r="J62">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>42415</v>
+        <v>42454</v>
       </c>
       <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63">
+        <v>50</v>
+      </c>
+      <c r="D63">
+        <v>30</v>
+      </c>
+      <c r="E63" s="6">
+        <v>27</v>
+      </c>
+      <c r="F63" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="G63" s="6">
+        <v>24</v>
+      </c>
+      <c r="H63" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I63">
+        <v>4.5</v>
+      </c>
+      <c r="J63">
         <v>4</v>
-      </c>
-      <c r="C63">
-        <v>51</v>
-      </c>
-      <c r="D63">
-        <v>32</v>
-      </c>
-      <c r="E63" s="6">
-        <v>35</v>
-      </c>
-      <c r="F63" s="6">
-        <v>7</v>
-      </c>
-      <c r="G63" s="6">
-        <v>17</v>
-      </c>
-      <c r="H63" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I63" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J63">
-        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>42454</v>
+        <v>42505</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C64">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D64">
         <v>30</v>
       </c>
       <c r="E64" s="6">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F64" s="6">
-        <v>10.5</v>
-      </c>
-      <c r="G64" s="6">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="G64">
+        <v>20</v>
       </c>
       <c r="H64" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I64">
-        <v>4.5</v>
-      </c>
-      <c r="J64">
-        <v>4</v>
+      <c r="I64" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J64" s="6">
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>42505</v>
+        <v>42515</v>
       </c>
       <c r="B65" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C65">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D65">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E65" s="6">
-        <v>34</v>
+        <v>25.5</v>
       </c>
       <c r="F65" s="6">
-        <v>7</v>
-      </c>
-      <c r="G65">
-        <v>20</v>
+        <v>2.5</v>
+      </c>
+      <c r="G65" s="6">
+        <v>28</v>
       </c>
       <c r="H65" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I65" t="e">
-        <v>#N/A</v>
+      <c r="I65">
+        <v>5</v>
       </c>
       <c r="J65" s="6">
-        <v>9</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>42515</v>
+        <v>42597</v>
       </c>
       <c r="B66" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C66">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D66">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E66" s="6">
-        <v>25.5</v>
+        <v>38</v>
       </c>
       <c r="F66" s="6">
-        <v>2.5</v>
+        <v>7</v>
       </c>
       <c r="G66" s="6">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="H66" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I66">
-        <v>5</v>
+      <c r="I66" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J66" s="6">
-        <v>1.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>42597</v>
+        <v>42602</v>
       </c>
       <c r="B67" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C67">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D67">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E67" s="6">
-        <v>38</v>
+        <v>24.5</v>
       </c>
       <c r="F67" s="6">
-        <v>7</v>
+        <v>9.5</v>
       </c>
       <c r="G67" s="6">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H67" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I67" t="e">
-        <v>#N/A</v>
+      <c r="I67">
+        <v>5.5</v>
       </c>
       <c r="J67" s="6">
-        <v>9</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>42602</v>
+        <v>42626</v>
       </c>
       <c r="B68" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C68">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D68">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E68" s="6">
-        <v>24.5</v>
+        <v>27</v>
       </c>
       <c r="F68" s="6">
-        <v>9.5</v>
+        <v>7</v>
       </c>
       <c r="G68" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H68" t="e">
         <v>#N/A</v>
       </c>
       <c r="I68">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="J68" s="6">
-        <v>2.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>42626</v>
+        <v>42644</v>
       </c>
       <c r="B69" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C69">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D69">
-        <v>35</v>
+        <v>36.5</v>
       </c>
       <c r="E69" s="6">
-        <v>27</v>
+        <v>24.5</v>
       </c>
       <c r="F69" s="6">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G69" s="6">
-        <v>22</v>
+        <v>19.5</v>
       </c>
       <c r="H69" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I69">
-        <v>5</v>
+      <c r="I69" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J69" s="6">
-        <v>4</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>42644</v>
+        <v>42689</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C70">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D70">
-        <v>36.5</v>
+        <v>38</v>
       </c>
       <c r="E70" s="6">
-        <v>24.5</v>
+        <v>36</v>
       </c>
       <c r="F70" s="6">
-        <v>11</v>
-      </c>
-      <c r="G70" s="6">
-        <v>19.5</v>
+        <v>9</v>
+      </c>
+      <c r="G70" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H70" t="e">
         <v>#N/A</v>
@@ -2763,30 +2763,30 @@
         <v>#N/A</v>
       </c>
       <c r="J70" s="6">
-        <v>8.5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>42689</v>
+        <v>42781</v>
       </c>
       <c r="B71" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C71">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D71">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E71" s="6">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F71" s="6">
-        <v>9</v>
-      </c>
-      <c r="G71" t="e">
-        <v>#N/A</v>
+        <v>6</v>
+      </c>
+      <c r="G71" s="6">
+        <v>18</v>
       </c>
       <c r="H71" t="e">
         <v>#N/A</v>
@@ -2795,12 +2795,12 @@
         <v>#N/A</v>
       </c>
       <c r="J71" s="6">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>42781</v>
+        <v>42870</v>
       </c>
       <c r="B72" t="s">
         <v>4</v>
@@ -2809,16 +2809,16 @@
         <v>52</v>
       </c>
       <c r="D72">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E72" s="6">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F72" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G72" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H72" t="e">
         <v>#N/A</v>
@@ -2827,30 +2827,30 @@
         <v>#N/A</v>
       </c>
       <c r="J72" s="6">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>42870</v>
+        <v>42889</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C73">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D73">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E73" s="6">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F73" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G73" s="6">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H73" t="e">
         <v>#N/A</v>
@@ -2859,30 +2859,30 @@
         <v>#N/A</v>
       </c>
       <c r="J73" s="6">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>42889</v>
+        <v>42962</v>
       </c>
       <c r="B74" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C74">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D74">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E74" s="6">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F74" s="6">
         <v>6</v>
       </c>
       <c r="G74" s="6">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H74" t="e">
         <v>#N/A</v>
@@ -2891,30 +2891,30 @@
         <v>#N/A</v>
       </c>
       <c r="J74" s="6">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>42962</v>
+        <v>43054</v>
       </c>
       <c r="B75" t="s">
-        <v>4</v>
-      </c>
-      <c r="C75">
-        <v>52</v>
+        <v>2</v>
+      </c>
+      <c r="C75" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D75">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E75" s="6">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F75" s="6">
         <v>6</v>
       </c>
       <c r="G75" s="6">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="H75" t="e">
         <v>#N/A</v>
@@ -2923,7 +2923,7 @@
         <v>#N/A</v>
       </c>
       <c r="J75" s="6">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -2931,22 +2931,22 @@
         <v>43054</v>
       </c>
       <c r="B76" t="s">
-        <v>2</v>
-      </c>
-      <c r="C76" t="e">
-        <v>#N/A</v>
+        <v>4</v>
+      </c>
+      <c r="C76">
+        <v>51</v>
       </c>
       <c r="D76">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E76" s="6">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F76" s="6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G76" s="6">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="H76" t="e">
         <v>#N/A</v>
@@ -2960,25 +2960,25 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>43054</v>
+        <v>43112</v>
       </c>
       <c r="B77" t="s">
-        <v>4</v>
-      </c>
-      <c r="C77">
-        <v>51</v>
+        <v>10</v>
+      </c>
+      <c r="C77" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D77">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E77" s="6">
-        <v>34</v>
+        <v>23.5</v>
       </c>
       <c r="F77" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G77" s="6">
-        <v>22</v>
+        <v>28.5</v>
       </c>
       <c r="H77" t="e">
         <v>#N/A</v>
@@ -2987,30 +2987,30 @@
         <v>#N/A</v>
       </c>
       <c r="J77" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>43112</v>
+        <v>43129</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C78" t="e">
         <v>#N/A</v>
       </c>
       <c r="D78">
-        <v>32</v>
+        <v>33.4</v>
       </c>
       <c r="E78" s="6">
-        <v>23.5</v>
+        <v>26.1</v>
       </c>
       <c r="F78" s="6">
-        <v>9</v>
+        <v>5.5</v>
       </c>
       <c r="G78" s="6">
-        <v>28.5</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="H78" t="e">
         <v>#N/A</v>
@@ -3019,30 +3019,30 @@
         <v>#N/A</v>
       </c>
       <c r="J78" s="6">
-        <v>7</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>43129</v>
+        <v>43159</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C79" t="e">
         <v>#N/A</v>
       </c>
       <c r="D79">
-        <v>33.4</v>
+        <v>32</v>
       </c>
       <c r="E79" s="6">
-        <v>26.1</v>
+        <v>30</v>
       </c>
       <c r="F79" s="6">
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="G79" s="6">
-        <v>17.600000000000001</v>
+        <v>21</v>
       </c>
       <c r="H79" t="e">
         <v>#N/A</v>
@@ -3051,12 +3051,12 @@
         <v>#N/A</v>
       </c>
       <c r="J79" s="6">
-        <v>9.1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>43159</v>
+        <v>43173</v>
       </c>
       <c r="B80" t="s">
         <v>2</v>
@@ -3065,16 +3065,16 @@
         <v>#N/A</v>
       </c>
       <c r="D80">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E80" s="6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F80" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G80" s="6">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H80" t="e">
         <v>#N/A</v>
@@ -3088,13 +3088,13 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>43173</v>
+        <v>43174</v>
       </c>
       <c r="B81" t="s">
-        <v>2</v>
-      </c>
-      <c r="C81" t="e">
-        <v>#N/A</v>
+        <v>9</v>
+      </c>
+      <c r="C81">
+        <v>52</v>
       </c>
       <c r="D81">
         <v>34</v>
@@ -3106,7 +3106,7 @@
         <v>8</v>
       </c>
       <c r="G81" s="6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H81" t="e">
         <v>#N/A</v>
@@ -3115,30 +3115,30 @@
         <v>#N/A</v>
       </c>
       <c r="J81" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>43174</v>
+        <v>43540</v>
       </c>
       <c r="B82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C82">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D82">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E82" s="6">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F82" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G82" s="6">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="H82" t="e">
         <v>#N/A</v>
@@ -3147,24 +3147,24 @@
         <v>#N/A</v>
       </c>
       <c r="J82" s="6">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>43540</v>
+        <v>43903</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
       </c>
       <c r="C83">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D83">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E83" s="6">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F83" s="6">
         <v>7</v>
@@ -3179,30 +3179,30 @@
         <v>#N/A</v>
       </c>
       <c r="J83" s="6">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>43903</v>
+        <v>44053</v>
       </c>
       <c r="B84" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C84">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D84">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E84" s="6">
-        <v>38</v>
-      </c>
-      <c r="F84" s="6">
-        <v>7</v>
-      </c>
-      <c r="G84" s="6">
-        <v>7</v>
+        <v>32</v>
+      </c>
+      <c r="F84" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G84" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H84" t="e">
         <v>#N/A</v>
@@ -3210,31 +3210,31 @@
       <c r="I84" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J84" s="6">
-        <v>5</v>
+      <c r="J84" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>44053</v>
+        <v>44092</v>
       </c>
       <c r="B85" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C85">
+        <v>47</v>
+      </c>
+      <c r="D85">
         <v>46</v>
       </c>
-      <c r="D85">
-        <v>44</v>
-      </c>
       <c r="E85" s="6">
-        <v>32</v>
-      </c>
-      <c r="F85" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G85" t="e">
-        <v>#N/A</v>
+        <v>35</v>
+      </c>
+      <c r="F85" s="6">
+        <v>10</v>
+      </c>
+      <c r="G85" s="6">
+        <v>5</v>
       </c>
       <c r="H85" t="e">
         <v>#N/A</v>
@@ -3242,47 +3242,15 @@
       <c r="I85" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J85" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <v>44092</v>
-      </c>
-      <c r="B86" t="s">
-        <v>8</v>
-      </c>
-      <c r="C86">
-        <v>47</v>
-      </c>
-      <c r="D86">
-        <v>46</v>
-      </c>
-      <c r="E86" s="6">
-        <v>35</v>
-      </c>
-      <c r="F86" s="6">
-        <v>10</v>
-      </c>
-      <c r="G86" s="6">
-        <v>5</v>
-      </c>
-      <c r="H86" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I86" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J86" s="6">
+      <c r="J85" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I118" s="5"/>
-    </row>
-    <row r="148" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H148" s="4"/>
+    <row r="117" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I117" s="5"/>
+    </row>
+    <row r="147" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H147" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
SA newspoll in records only
</commit_message>
<xml_diff>
--- a/python/Data/poll-data-sa.xlsx
+++ b/python/Data/poll-data-sa.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\python\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5413D5-EAE9-4D3B-A00F-82514EF7C1E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FABC824-652B-4E44-933D-9EF5514E8198}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="30" windowWidth="12480" windowHeight="8295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="375" yWindow="5205" windowWidth="30180" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="17">
   <si>
     <t>MidDate</t>
   </si>
@@ -410,12 +410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="600" activePane="bottomLeft"/>
+      <pane ySplit="600" topLeftCell="A71" activePane="bottomLeft"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3246,6 +3247,38 @@
         <v>4</v>
       </c>
     </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>44254</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86">
+        <v>49</v>
+      </c>
+      <c r="D86">
+        <v>43</v>
+      </c>
+      <c r="E86" s="6">
+        <v>36</v>
+      </c>
+      <c r="F86" s="6">
+        <v>10</v>
+      </c>
+      <c r="G86" s="6">
+        <v>6</v>
+      </c>
+      <c r="H86" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I86" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J86" s="6">
+        <v>5</v>
+      </c>
+    </row>
     <row r="117" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I117" s="5"/>
     </row>

</xml_diff>